<commit_message>
update for issue #407, testing next
</commit_message>
<xml_diff>
--- a/programs/frameworks/neural/data/kvm.xlsx
+++ b/programs/frameworks/neural/data/kvm.xlsx
@@ -8,18 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\objec\Documents\Code\objeck-lang\programs\frameworks\neural\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21E971E-0E49-4C63-BE94-AA46F4039E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F79337A-9F85-4824-B4AE-1F2A7AFB36D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="1728" windowWidth="19932" windowHeight="13332" xr2:uid="{FB11F44C-8569-4840-B176-A127A7EB8F39}"/>
+    <workbookView xWindow="6804" yWindow="1692" windowWidth="20616" windowHeight="14472" xr2:uid="{FB11F44C-8569-4840-B176-A127A7EB8F39}"/>
   </bookViews>
   <sheets>
-    <sheet name="Model" sheetId="1" r:id="rId1"/>
+    <sheet name="Model (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="Model" sheetId="1" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Model!$D$2:$D$13</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Model!$E$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Model!$E$2:$E$13</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="6">
   <si>
     <t>x-point</t>
   </si>
@@ -114,6 +110,466 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.70455010969469E-2"/>
+          <c:y val="1.7386893589868217E-2"/>
+          <c:w val="0.88112481752084082"/>
+          <c:h val="0.89174337538292048"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>normal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Model (2)'!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Model (2)'!$E$2:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D985-42A0-901A-0C8733A0000F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>above</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Model (2)'!$B$16:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Model (2)'!$C$16:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D985-42A0-901A-0C8733A0000F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>below</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Model (2)'!$B$30:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Model (2)'!$C$30:$C$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D985-42A0-901A-0C8733A0000F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="155385136"/>
+        <c:axId val="797484495"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="155385136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="11"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="797484495"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+        <c:minorUnit val="0.5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="797484495"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="11"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="155385136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+        <c:minorUnit val="0.5"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -757,6 +1213,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1273,7 +1769,566 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>608596</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>3620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A57E63B-E319-41E5-AA1C-C06BD07DF9D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noChangeAspect="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1612,11 +2667,178 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E4B648-183E-4A47-9054-5B4F0ABC1F02}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <f>-2</f>
+        <v>-2</v>
+      </c>
+      <c r="B2">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>IF($A$2,-($B$2/$A$2),0)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <f>$C$2*D2+$B$2</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <f>ROW(D1)</f>
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>$C$2*D3+$B$2</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <f t="shared" ref="D4:D13" si="0">ROW(D2)</f>
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f>$C$2*D4+$B$2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <f>$C$2*D5+$B$2</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <f>$C$2*D6+$B$2</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <f>$C$2*D7+$B$2</f>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <f>$C$2*D8+$B$2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <f>$C$2*D9+$B$2</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <f>$C$2*D10+$B$2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <f>$C$2*D11+$B$2</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <f>$C$2*D12+$B$2</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <f>$C$2*D13+$B$2</f>
+        <v>6.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ECFAC71-496C-4039-BF62-D54991C20F2C}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1704,7 +2926,7 @@
         <v>0.5</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D13" si="3">ROW(D2)</f>
+        <f>ROW(D2)</f>
         <v>2</v>
       </c>
       <c r="E4">
@@ -1726,7 +2948,7 @@
         <v>0.5</v>
       </c>
       <c r="D5">
-        <f t="shared" si="3"/>
+        <f>ROW(D3)</f>
         <v>3</v>
       </c>
       <c r="E5">
@@ -1748,7 +2970,7 @@
         <v>0.5</v>
       </c>
       <c r="D6">
-        <f t="shared" si="3"/>
+        <f>ROW(D4)</f>
         <v>4</v>
       </c>
       <c r="E6">
@@ -1770,7 +2992,7 @@
         <v>0.5</v>
       </c>
       <c r="D7">
-        <f t="shared" si="3"/>
+        <f>ROW(D5)</f>
         <v>5</v>
       </c>
       <c r="E7">
@@ -1792,7 +3014,7 @@
         <v>0.5</v>
       </c>
       <c r="D8">
-        <f t="shared" si="3"/>
+        <f>ROW(D6)</f>
         <v>6</v>
       </c>
       <c r="E8">
@@ -1814,7 +3036,7 @@
         <v>0.5</v>
       </c>
       <c r="D9">
-        <f t="shared" si="3"/>
+        <f>ROW(D7)</f>
         <v>7</v>
       </c>
       <c r="E9">
@@ -1836,7 +3058,7 @@
         <v>0.5</v>
       </c>
       <c r="D10">
-        <f t="shared" si="3"/>
+        <f>ROW(D8)</f>
         <v>8</v>
       </c>
       <c r="E10">
@@ -1858,7 +3080,7 @@
         <v>0.5</v>
       </c>
       <c r="D11">
-        <f t="shared" si="3"/>
+        <f>ROW(D9)</f>
         <v>9</v>
       </c>
       <c r="E11">
@@ -1876,11 +3098,11 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:C13" si="4">-(B12/A12)</f>
+        <f t="shared" ref="C12:C13" si="3">-(B12/A12)</f>
         <v>0.5</v>
       </c>
       <c r="D12">
-        <f t="shared" si="3"/>
+        <f>ROW(D10)</f>
         <v>10</v>
       </c>
       <c r="E12">
@@ -1898,11 +3120,11 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="D13">
-        <f t="shared" si="3"/>
+        <f>ROW(D11)</f>
         <v>11</v>
       </c>
       <c r="E13">
@@ -1947,7 +3169,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <f>C16*D16+B16</f>
+        <f t="shared" ref="E16:E27" si="4">C16*D16+B16</f>
         <v>0.5</v>
       </c>
       <c r="F16">
@@ -1972,7 +3194,7 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <f>C17*D17+B17</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -1994,7 +3216,7 @@
         <v>2</v>
       </c>
       <c r="E18">
-        <f>C18*D18+B18</f>
+        <f t="shared" si="4"/>
         <v>1.5</v>
       </c>
     </row>
@@ -2016,7 +3238,7 @@
         <v>3</v>
       </c>
       <c r="E19">
-        <f>C19*D19+B19</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -2038,7 +3260,7 @@
         <v>4</v>
       </c>
       <c r="E20">
-        <f>C20*D20+B20</f>
+        <f t="shared" si="4"/>
         <v>2.5</v>
       </c>
     </row>
@@ -2060,7 +3282,7 @@
         <v>5</v>
       </c>
       <c r="E21">
-        <f>C21*D21+B21</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
@@ -2082,7 +3304,7 @@
         <v>6</v>
       </c>
       <c r="E22">
-        <f>C22*D22+B22</f>
+        <f t="shared" si="4"/>
         <v>3.5</v>
       </c>
     </row>
@@ -2104,7 +3326,7 @@
         <v>7</v>
       </c>
       <c r="E23">
-        <f>C23*D23+B23</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
     </row>
@@ -2126,7 +3348,7 @@
         <v>8</v>
       </c>
       <c r="E24">
-        <f>C24*D24+B24</f>
+        <f t="shared" si="4"/>
         <v>4.5</v>
       </c>
     </row>
@@ -2148,7 +3370,7 @@
         <v>9</v>
       </c>
       <c r="E25">
-        <f>C25*D25+B25</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -2170,7 +3392,7 @@
         <v>10</v>
       </c>
       <c r="E26">
-        <f>C26*D26+B26</f>
+        <f t="shared" si="4"/>
         <v>5.5</v>
       </c>
     </row>
@@ -2192,7 +3414,7 @@
         <v>11</v>
       </c>
       <c r="E27">
-        <f>C27*D27+B27</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
     </row>
@@ -2233,7 +3455,7 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <f>C30*D30+B30</f>
+        <f t="shared" ref="E30:E41" si="9">C30*D30+B30</f>
         <v>1.5</v>
       </c>
       <c r="F30">
@@ -2242,15 +3464,15 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
-        <f t="shared" ref="A31:A41" si="9">-2*F$30</f>
+        <f t="shared" ref="A31:A41" si="10">-2*F$30</f>
         <v>-3</v>
       </c>
       <c r="B31">
-        <f t="shared" ref="B31:B41" si="10">1*F$30</f>
+        <f t="shared" ref="B31:B41" si="11">1*F$30</f>
         <v>1.5</v>
       </c>
       <c r="C31">
-        <f t="shared" ref="C31:C41" si="11">-(B31/A31)</f>
+        <f t="shared" ref="C31:C41" si="12">-(B31/A31)</f>
         <v>0.5</v>
       </c>
       <c r="D31">
@@ -2258,227 +3480,227 @@
         <v>1</v>
       </c>
       <c r="E31">
-        <f>C31*D31+B31</f>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
+        <f t="shared" si="10"/>
+        <v>-3</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="11"/>
+        <v>1.5</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="D32">
+        <f t="shared" ref="D32:D41" si="13">ROW(D2)</f>
+        <v>2</v>
+      </c>
+      <c r="E32">
         <f t="shared" si="9"/>
-        <v>-3</v>
-      </c>
-      <c r="B32">
-        <f t="shared" si="10"/>
-        <v>1.5</v>
-      </c>
-      <c r="C32">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
-      </c>
-      <c r="D32">
-        <f t="shared" ref="D32:D41" si="12">ROW(D2)</f>
-        <v>2</v>
-      </c>
-      <c r="E32">
-        <f>C32*D32+B32</f>
         <v>2.5</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
+        <f t="shared" si="10"/>
+        <v>-3</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="11"/>
+        <v>1.5</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="E33">
         <f t="shared" si="9"/>
-        <v>-3</v>
-      </c>
-      <c r="B33">
-        <f t="shared" si="10"/>
-        <v>1.5</v>
-      </c>
-      <c r="C33">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="12"/>
-        <v>3</v>
-      </c>
-      <c r="E33">
-        <f>C33*D33+B33</f>
         <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
+        <f t="shared" si="10"/>
+        <v>-3</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="11"/>
+        <v>1.5</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="13"/>
+        <v>4</v>
+      </c>
+      <c r="E34">
         <f t="shared" si="9"/>
-        <v>-3</v>
-      </c>
-      <c r="B34">
-        <f t="shared" si="10"/>
-        <v>1.5</v>
-      </c>
-      <c r="C34">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="E34">
-        <f>C34*D34+B34</f>
         <v>3.5</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
+        <f t="shared" si="10"/>
+        <v>-3</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="11"/>
+        <v>1.5</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="E35">
         <f t="shared" si="9"/>
-        <v>-3</v>
-      </c>
-      <c r="B35">
-        <f t="shared" si="10"/>
-        <v>1.5</v>
-      </c>
-      <c r="C35">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
-      </c>
-      <c r="D35">
-        <f t="shared" si="12"/>
-        <v>5</v>
-      </c>
-      <c r="E35">
-        <f>C35*D35+B35</f>
         <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
+        <f t="shared" si="10"/>
+        <v>-3</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="11"/>
+        <v>1.5</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="13"/>
+        <v>6</v>
+      </c>
+      <c r="E36">
         <f t="shared" si="9"/>
-        <v>-3</v>
-      </c>
-      <c r="B36">
-        <f t="shared" si="10"/>
-        <v>1.5</v>
-      </c>
-      <c r="C36">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
-      </c>
-      <c r="D36">
-        <f t="shared" si="12"/>
-        <v>6</v>
-      </c>
-      <c r="E36">
-        <f>C36*D36+B36</f>
         <v>4.5</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
+        <f t="shared" si="10"/>
+        <v>-3</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="11"/>
+        <v>1.5</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="E37">
         <f t="shared" si="9"/>
-        <v>-3</v>
-      </c>
-      <c r="B37">
-        <f t="shared" si="10"/>
-        <v>1.5</v>
-      </c>
-      <c r="C37">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="12"/>
-        <v>7</v>
-      </c>
-      <c r="E37">
-        <f>C37*D37+B37</f>
         <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
+        <f t="shared" si="10"/>
+        <v>-3</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="11"/>
+        <v>1.5</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="E38">
         <f t="shared" si="9"/>
-        <v>-3</v>
-      </c>
-      <c r="B38">
-        <f t="shared" si="10"/>
-        <v>1.5</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="12"/>
-        <v>8</v>
-      </c>
-      <c r="E38">
-        <f>C38*D38+B38</f>
         <v>5.5</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
+        <f t="shared" si="10"/>
+        <v>-3</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="11"/>
+        <v>1.5</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="E39">
         <f t="shared" si="9"/>
-        <v>-3</v>
-      </c>
-      <c r="B39">
-        <f t="shared" si="10"/>
-        <v>1.5</v>
-      </c>
-      <c r="C39">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="12"/>
-        <v>9</v>
-      </c>
-      <c r="E39">
-        <f>C39*D39+B39</f>
         <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
+        <f t="shared" si="10"/>
+        <v>-3</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="11"/>
+        <v>1.5</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="E40">
         <f t="shared" si="9"/>
-        <v>-3</v>
-      </c>
-      <c r="B40">
-        <f t="shared" si="10"/>
-        <v>1.5</v>
-      </c>
-      <c r="C40">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
-      </c>
-      <c r="D40">
-        <f t="shared" si="12"/>
-        <v>10</v>
-      </c>
-      <c r="E40">
-        <f>C40*D40+B40</f>
         <v>6.5</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
+        <f t="shared" si="10"/>
+        <v>-3</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="11"/>
+        <v>1.5</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="12"/>
+        <v>0.5</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="13"/>
+        <v>11</v>
+      </c>
+      <c r="E41">
         <f t="shared" si="9"/>
-        <v>-3</v>
-      </c>
-      <c r="B41">
-        <f t="shared" si="10"/>
-        <v>1.5</v>
-      </c>
-      <c r="C41">
-        <f t="shared" si="11"/>
-        <v>0.5</v>
-      </c>
-      <c r="D41">
-        <f t="shared" si="12"/>
-        <v>11</v>
-      </c>
-      <c r="E41">
-        <f>C41*D41+B41</f>
         <v>7</v>
       </c>
     </row>

</xml_diff>